<commit_message>
fix update prgress template
</commit_message>
<xml_diff>
--- a/public/files/templates/update_progress_template.xlsx
+++ b/public/files/templates/update_progress_template.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10613"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10909"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hazem/code/cost-control/public/files/templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5BA2D0F-8E4A-CC40-B08F-8E97484C1EDD}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE49B757-EF7D-3946-A281-3784D78F0ABD}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="29000" yWindow="2860" windowWidth="25040" windowHeight="14500" xr2:uid="{0346A8DA-54F5-D243-9ADE-C83E7D7DA5A4}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>Activity Code</t>
   </si>
@@ -34,6 +34,9 @@
   </si>
   <si>
     <t>Progress</t>
+  </si>
+  <si>
+    <t>Activity Name</t>
   </si>
 </sst>
 </file>
@@ -403,7 +406,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D5F19C6-0810-7746-8BFA-DF123D781737}">
-  <dimension ref="A1:C1"/>
+  <dimension ref="A1:D1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
@@ -412,18 +415,21 @@
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="22.6640625" style="4" customWidth="1"/>
-    <col min="2" max="2" width="24" style="4" customWidth="1"/>
-    <col min="3" max="3" width="16" style="2" customWidth="1"/>
+    <col min="2" max="3" width="24" style="4" customWidth="1"/>
+    <col min="4" max="4" width="16" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
     </row>

</xml_diff>